<commit_message>
Added Use Case Review Logs
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint2/Burndown Chart.xlsx
+++ b/Project/Phase 2/Sprint2/Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmtbl\Documents\GitHub\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafa\Desktop\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C280AD75-F58E-4F33-83BA-662FF86B2BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E005976-7435-49E0-9289-31404E4EE2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,11 +75,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -95,9 +102,12 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -168,61 +178,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -274,74 +234,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -364,7 +425,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -450,33 +511,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$I$8</c:f>
+              <c:f>Sheet1!$B$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,30 +597,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$I$9</c:f>
+              <c:f>Sheet1!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>3.8000000000000003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2571428571428571</c:v>
+                  <c:v>5.1428571428571432</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7142857142857144</c:v>
+                  <c:v>4.2857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1714285714285717</c:v>
+                  <c:v>3.4285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6285714285714286</c:v>
+                  <c:v>2.5714285714285716</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0857142857142859</c:v>
+                  <c:v>1.7142857142857144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5428571428571427</c:v>
+                  <c:v>0.85714285714285765</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -629,7 +690,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="236351578"/>
@@ -694,7 +755,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1519336200"/>
@@ -717,7 +778,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -738,9 +799,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4371975" cy="2714625"/>
     <xdr:graphicFrame macro="">
@@ -967,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -981,7 +1042,7 @@
     <col min="10" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1">
         <v>44891</v>
       </c>
@@ -1004,299 +1065,298 @@
         <v>44897</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="12">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="12">
         <v>2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="12">
         <v>3</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="12">
         <v>4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="12">
         <v>5</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="12">
         <v>6</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="12">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+    <row r="7" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="14">
+        <f>SUM(B3:B6)</f>
+        <v>6</v>
+      </c>
+      <c r="C7" s="14">
+        <f t="shared" ref="C7:I7" si="0">B7-SUM(C3:C6)</f>
+        <v>6</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6">
-        <f>SUM(B3:B7)</f>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="C8" s="6">
-        <f t="shared" ref="C8:I8" si="0">B8-SUM(C3:C7)</f>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="D8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="E8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="F8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8000000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="8">
-        <f>SUM(B3:B7)</f>
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="C9" s="9">
-        <f>B9-(B9/7*C2)</f>
-        <v>3.2571428571428571</v>
-      </c>
-      <c r="D9" s="9">
-        <f t="shared" ref="D9:I9" si="1">$B9-($B9/7*D2)</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="B8" s="16">
+        <f>SUM(B3:B6)</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="17">
+        <f>B8-(B8/7*C2)</f>
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="D8" s="17">
+        <f t="shared" ref="D8:I8" si="1">$B8-($B8/7*D2)</f>
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="E8" s="17">
         <f t="shared" si="1"/>
-        <v>2.1714285714285717</v>
-      </c>
-      <c r="F9" s="9">
+        <v>3.4285714285714288</v>
+      </c>
+      <c r="F8" s="17">
         <f t="shared" si="1"/>
-        <v>1.6285714285714286</v>
-      </c>
-      <c r="G9" s="9">
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="G8" s="17">
         <f t="shared" si="1"/>
-        <v>1.0857142857142859</v>
-      </c>
-      <c r="H9" s="9">
+        <v>1.7142857142857144</v>
+      </c>
+      <c r="H8" s="17">
         <f t="shared" si="1"/>
-        <v>0.5428571428571427</v>
-      </c>
-      <c r="I9" s="9">
+        <v>0.85714285714285765</v>
+      </c>
+      <c r="I8" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+    <row r="9" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+    <row r="10" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+    <row r="11" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+    <row r="12" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="P12" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+    <row r="13" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
+      <c r="B14" s="24"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="D15" s="15" t="s">
+      <c r="B15" s="26"/>
+      <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+    <row r="16" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="D16" s="16" t="s">
+      <c r="B16" s="28"/>
+      <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="D17" s="17" t="s">
+      <c r="B17" s="30"/>
+      <c r="D17" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="D18" s="18" t="s">
+      <c r="B18" s="32"/>
+      <c r="D18" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="D19" s="19" t="s">
+      <c r="B19" s="22"/>
+      <c r="D19" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="19"/>
+    </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2284,7 +2344,7 @@
     <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 1 Metric and 1 Use Case Review and updated Scrum files accordingly
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint2/Burndown Chart.xlsx
+++ b/Project/Phase 2/Sprint2/Burndown Chart.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafa\Desktop\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E005976-7435-49E0-9289-31404E4EE2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D1BC1D-E08A-4EB9-8578-6C43BBCC2312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,18 +68,25 @@
     <t>Pedro Lopes</t>
   </si>
   <si>
-    <t>1,2,3,4,5</t>
+    <t>1,2,3,4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,86 +332,87 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +489,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$I$2</c:f>
+              <c:f>'Burndown Chart'!$C$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -511,7 +519,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$I$7</c:f>
+              <c:f>'Burndown Chart'!$B$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -531,13 +539,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,7 +575,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$I$2</c:f>
+              <c:f>'Burndown Chart'!$C$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -597,7 +605,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$I$8</c:f>
+              <c:f>'Burndown Chart'!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1031,7 +1039,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1113,9 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10">
+        <v>0.2</v>
+      </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
@@ -1150,7 +1160,9 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10">
+        <v>0.2</v>
+      </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
     </row>
@@ -1180,15 +1192,15 @@
       </c>
       <c r="G7" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="H7" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="I7" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1260,6 +1272,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
Updated burndown Chart and Scrum master log
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint2/Burndown Chart.xlsx
+++ b/Project/Phase 2/Sprint2/Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Ambiente de Trabalho\PC\Faculdade\3ANO\1Semestre\ES\Projeto\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A035A3B5-ADFE-45C3-A496-496CFB35BAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48C1779-FD05-4E78-8A93-6E34F05BC253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -393,6 +393,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -429,7 +430,6 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1069,25 +1069,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="1">
-        <v>44891</v>
+        <v>44870</v>
       </c>
       <c r="D1" s="1">
-        <v>44892</v>
+        <v>44871</v>
       </c>
       <c r="E1" s="1">
-        <v>44893</v>
+        <v>44872</v>
       </c>
       <c r="F1" s="1">
-        <v>44894</v>
+        <v>44873</v>
       </c>
       <c r="G1" s="1">
-        <v>44895</v>
+        <v>44874</v>
       </c>
       <c r="H1" s="1">
-        <v>44896</v>
+        <v>44875</v>
       </c>
       <c r="I1" s="1">
-        <v>44897</v>
+        <v>44876</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1386,10 +1386,10 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="25"/>
+      <c r="B19" s="26"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1398,10 +1398,10 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="28"/>
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
@@ -1412,10 +1412,10 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="30"/>
       <c r="D21" s="6" t="s">
         <v>6</v>
       </c>
@@ -1426,28 +1426,28 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="31"/>
+      <c r="B22" s="32"/>
       <c r="D22" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="34"/>
       <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="24"/>
       <c r="D24" s="9" t="s">
         <v>9</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
+      <c r="A28" s="22"/>
       <c r="D28" s="19"/>
     </row>
     <row r="29" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>